<commit_message>
[IMP] Adjust GL Project
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_gl_project.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_gl_project.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="80">
   <si>
     <t xml:space="preserve">Project Report</t>
   </si>
@@ -58,6 +58,9 @@
     <t xml:space="preserve">Activity</t>
   </si>
   <si>
+    <t xml:space="preserve">Charge Type</t>
+  </si>
+  <si>
     <t xml:space="preserve">Budget View</t>
   </si>
   <si>
@@ -83,9 +86,6 @@
   </si>
   <si>
     <t xml:space="preserve">Run Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Charge Type</t>
   </si>
   <si>
     <t xml:space="preserve">Fund Rule - Expense Group</t>
@@ -434,7 +434,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BJ21"/>
+  <dimension ref="A1:BJ22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -726,10 +726,10 @@
       <c r="BE12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="8"/>
+      <c r="B13" s="6"/>
       <c r="C13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -852,6 +852,10 @@
       <c r="BE19" s="3"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="8"/>
       <c r="C20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
@@ -866,190 +870,204 @@
       <c r="BE20" s="3"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="12" t="s">
+      <c r="C21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="Z21" s="3"/>
+      <c r="AA21" s="3"/>
+      <c r="AB21" s="3"/>
+      <c r="AD21" s="3"/>
+      <c r="AJ21" s="3"/>
+      <c r="AV21" s="3"/>
+      <c r="AY21" s="3"/>
+      <c r="AZ21" s="3"/>
+      <c r="BE21" s="3"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C22" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D22" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E21" s="12" t="s">
+      <c r="E22" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="F21" s="12" t="s">
+      <c r="F22" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="G21" s="12" t="s">
+      <c r="G22" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="H21" s="12" t="s">
+      <c r="H22" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="I21" s="12" t="s">
+      <c r="I22" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="J21" s="12" t="s">
+      <c r="J22" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="K21" s="12" t="s">
+      <c r="K22" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="L21" s="12" t="s">
+      <c r="L22" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="M21" s="12" t="s">
+      <c r="M22" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="N21" s="12" t="s">
+      <c r="N22" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="O21" s="12" t="s">
+      <c r="O22" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="P21" s="12" t="s">
+      <c r="P22" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="Q21" s="12" t="s">
+      <c r="Q22" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="R21" s="12" t="s">
+      <c r="R22" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="S21" s="12" t="s">
+      <c r="S22" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="T21" s="12" t="s">
+      <c r="T22" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="U21" s="12" t="s">
+      <c r="U22" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="V21" s="12" t="s">
+      <c r="V22" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="W21" s="12" t="s">
+      <c r="W22" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="X21" s="12" t="s">
+      <c r="X22" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="Y21" s="12" t="s">
+      <c r="Y22" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="Z21" s="12" t="s">
+      <c r="Z22" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="AA21" s="12" t="s">
+      <c r="AA22" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="AB21" s="12" t="s">
+      <c r="AB22" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="AC21" s="12" t="s">
+      <c r="AC22" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="AD21" s="12" t="s">
+      <c r="AD22" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="AE21" s="12" t="s">
+      <c r="AE22" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="AF21" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="AG21" s="12" t="s">
+      <c r="AF22" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG22" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="AH21" s="12" t="s">
+      <c r="AH22" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="AI21" s="12" t="s">
+      <c r="AI22" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="AJ21" s="12" t="s">
+      <c r="AJ22" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="AK21" s="12" t="s">
+      <c r="AK22" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="AL21" s="12" t="s">
+      <c r="AL22" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="AM21" s="12" t="s">
+      <c r="AM22" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="AN21" s="12" t="s">
+      <c r="AN22" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="AO21" s="12" t="s">
+      <c r="AO22" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="AP21" s="12" t="s">
+      <c r="AP22" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="AQ21" s="12" t="s">
+      <c r="AQ22" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="AR21" s="12" t="s">
+      <c r="AR22" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="AS21" s="12" t="s">
+      <c r="AS22" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="AT21" s="12" t="s">
+      <c r="AT22" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="AU21" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="AV21" s="12" t="s">
+      <c r="AU22" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="AV22" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="AW21" s="12" t="s">
+      <c r="AW22" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="AX21" s="12" t="s">
+      <c r="AX22" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="AY21" s="12" t="s">
+      <c r="AY22" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="AZ21" s="12" t="s">
+      <c r="AZ22" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="BA21" s="12" t="s">
+      <c r="BA22" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="BB21" s="12" t="s">
+      <c r="BB22" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="BC21" s="12" t="s">
+      <c r="BC22" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="BD21" s="12" t="s">
+      <c r="BD22" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="BE21" s="12" t="s">
+      <c r="BE22" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="BF21" s="12" t="s">
+      <c r="BF22" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="BG21" s="12" t="s">
+      <c r="BG22" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="BH21" s="12" t="s">
+      <c r="BH22" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="BI21" s="12" t="s">
+      <c r="BI22" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="BJ21" s="13" t="s">
+      <c r="BJ22" s="13" t="s">
         <v>79</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[IMP] Add tax code, vat amount, base amount and wht amount in GL Project
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_gl_project.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_gl_project.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="83">
   <si>
     <t xml:space="preserve">Project Report</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t xml:space="preserve">Run Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Noted for base amount, vat amount and wht amount</t>
   </si>
   <si>
     <t xml:space="preserve">Fund Rule - Expense Group</t>
@@ -275,7 +278,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -311,14 +314,8 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -335,6 +332,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFCCFFFF"/>
         <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF200"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -421,11 +424,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -442,6 +445,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFF200"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -450,7 +513,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BL22"/>
+  <dimension ref="A1:BZ22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -518,7 +581,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="62" min="62" style="0" width="20.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="63" min="63" style="0" width="17.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="64" style="0" width="25.98"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="65" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="75" min="65" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="76" min="76" style="0" width="18.61"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="77" min="77" style="0" width="19.17"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="78" min="78" style="0" width="24.73"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="79" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -899,202 +966,219 @@
       <c r="AZ21" s="3"/>
       <c r="BA21" s="3"/>
       <c r="BF21" s="3"/>
+      <c r="BX21" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="BY21" s="12"/>
+      <c r="BZ21" s="12"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" s="12" t="s">
+      <c r="B22" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E22" s="12" t="s">
+      <c r="D22" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="F22" s="12" t="s">
+      <c r="E22" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="G22" s="12" t="s">
+      <c r="F22" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="H22" s="12" t="s">
+      <c r="G22" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="I22" s="12" t="s">
+      <c r="H22" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="J22" s="12" t="s">
+      <c r="I22" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="K22" s="12" t="s">
+      <c r="J22" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="L22" s="12" t="s">
+      <c r="K22" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="M22" s="12" t="s">
+      <c r="L22" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="N22" s="12" t="s">
+      <c r="M22" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="O22" s="12" t="s">
+      <c r="N22" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="P22" s="12" t="s">
+      <c r="O22" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="Q22" s="12" t="s">
+      <c r="P22" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="R22" s="12" t="s">
+      <c r="Q22" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="S22" s="12" t="s">
+      <c r="R22" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="T22" s="12" t="s">
+      <c r="S22" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="U22" s="12" t="s">
+      <c r="T22" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="V22" s="12" t="s">
+      <c r="U22" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="W22" s="12" t="s">
+      <c r="V22" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="X22" s="12" t="s">
+      <c r="W22" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="Y22" s="12" t="s">
+      <c r="X22" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="Z22" s="12" t="s">
+      <c r="Y22" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="AA22" s="12" t="s">
+      <c r="Z22" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="AB22" s="12" t="s">
+      <c r="AA22" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="AC22" s="12" t="s">
+      <c r="AB22" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="AD22" s="12" t="s">
+      <c r="AC22" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="AE22" s="12" t="s">
+      <c r="AD22" s="13" t="s">
         <v>50</v>
       </c>
+      <c r="AE22" s="13" t="s">
+        <v>51</v>
+      </c>
       <c r="AF22" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="AG22" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="AG22" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="AH22" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="AI22" s="12" t="s">
+      <c r="AH22" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="AJ22" s="12" t="s">
+      <c r="AI22" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="AK22" s="12" t="s">
+      <c r="AJ22" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="AL22" s="12" t="s">
+      <c r="AK22" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="AM22" s="12" t="s">
+      <c r="AL22" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="AN22" s="12" t="s">
+      <c r="AM22" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="AO22" s="12" t="s">
+      <c r="AN22" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="AP22" s="12" t="s">
+      <c r="AO22" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="AQ22" s="12" t="s">
+      <c r="AP22" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="AR22" s="12" t="s">
+      <c r="AQ22" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="AS22" s="12" t="s">
+      <c r="AR22" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="AT22" s="12" t="s">
+      <c r="AS22" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="AU22" s="12" t="s">
+      <c r="AT22" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="AV22" s="12" t="s">
+      <c r="AU22" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="AV22" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="AW22" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="AX22" s="12" t="s">
+      <c r="AW22" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="AY22" s="12" t="s">
+      <c r="AX22" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="AZ22" s="12" t="s">
+      <c r="AY22" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="BA22" s="12" t="s">
+      <c r="AZ22" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="BB22" s="12" t="s">
+      <c r="BA22" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="BC22" s="12" t="s">
+      <c r="BB22" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="BD22" s="12" t="s">
+      <c r="BC22" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="BE22" s="12" t="s">
+      <c r="BD22" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="BF22" s="12" t="s">
+      <c r="BE22" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="BG22" s="12" t="s">
+      <c r="BF22" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="BH22" s="12" t="s">
+      <c r="BG22" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="BI22" s="12" t="s">
+      <c r="BH22" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="BJ22" s="12" t="s">
+      <c r="BI22" s="13" t="s">
         <v>79</v>
       </c>
+      <c r="BJ22" s="13" t="s">
+        <v>80</v>
+      </c>
       <c r="BK22" s="14" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="BL22" s="14" t="s">
-        <v>81</v>
+        <v>82</v>
+      </c>
+      <c r="BX22" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="BY22" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="BZ22" s="12" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="BX21:BZ21"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>